<commit_message>
fix: apply menu type enum to the all menu service codes
</commit_message>
<xml_diff>
--- a/hanseifood/assets/templates/excel_template.xlsx
+++ b/hanseifood/assets/templates/excel_template.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seungwoosmac/side_projects/univ_menu_web/back/hanseifood_back/hanseifood/assets/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC94B83-F729-FE4D-9157-A0C0758DDD0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6DAEE94-D04D-EC4F-B35D-BE5B3481D289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="-100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="12월3주" sheetId="1" r:id="rId1"/>
+    <sheet name="식단표" sheetId="1" r:id="rId1"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId2"/>
@@ -462,23 +462,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -492,6 +475,11 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -512,6 +500,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -16217,7 +16217,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12:E16"/>
+      <selection sqref="A1:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
@@ -16232,142 +16232,142 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A3" s="19"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
     </row>
     <row r="4" spans="1:8" s="1" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A4" s="20"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" s="4" customFormat="1" ht="20.25" customHeight="1">
       <c r="A5" s="3"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="25"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="21"/>
     </row>
     <row r="6" spans="1:8" s="4" customFormat="1" ht="26.25" customHeight="1">
       <c r="A6" s="5"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="26"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="22"/>
     </row>
     <row r="7" spans="1:8" ht="25" customHeight="1">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
       <c r="H7" s="6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="25" customHeight="1">
-      <c r="A8" s="16"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
+      <c r="A8" s="33"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
     </row>
     <row r="9" spans="1:8" ht="25" customHeight="1">
-      <c r="A9" s="16"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
+      <c r="A9" s="33"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
     </row>
     <row r="10" spans="1:8" ht="25" customHeight="1">
-      <c r="A10" s="16"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
+      <c r="A10" s="33"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
     </row>
     <row r="11" spans="1:8" ht="25" customHeight="1">
-      <c r="A11" s="17"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
+      <c r="A11" s="34"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
     </row>
     <row r="12" spans="1:8" ht="25" customHeight="1">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
     </row>
     <row r="13" spans="1:8" ht="25" customHeight="1">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
+      <c r="A13" s="19"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
     </row>
     <row r="14" spans="1:8" ht="25" customHeight="1">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
+      <c r="A14" s="19"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
     </row>
     <row r="15" spans="1:8" ht="25" customHeight="1">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
+      <c r="A15" s="19"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
     </row>
     <row r="16" spans="1:8" ht="25" customHeight="1">
-      <c r="A16" s="13"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
+      <c r="A16" s="20"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
     </row>
     <row r="17" spans="1:6" ht="28">
       <c r="A17" s="8" t="s">
@@ -16380,45 +16380,51 @@
       <c r="F17" s="9"/>
     </row>
     <row r="18" spans="1:6" ht="32.25" customHeight="1">
-      <c r="A18" s="27" t="s">
+      <c r="A18" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="32"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="34"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="30"/>
     </row>
     <row r="19" spans="1:6" ht="32.25" customHeight="1">
-      <c r="A19" s="28"/>
-      <c r="B19" s="30"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="31"/>
+      <c r="A19" s="24"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="27"/>
     </row>
     <row r="20" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A20" s="29" t="s">
+      <c r="A20" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="30"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="30"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="31"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="27"/>
     </row>
     <row r="21" spans="1:6" ht="32.25" customHeight="1">
-      <c r="A21" s="21" t="s">
+      <c r="A21" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="22"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="E7:E11"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="C7:C11"/>
+    <mergeCell ref="C12:C16"/>
+    <mergeCell ref="A7:A11"/>
     <mergeCell ref="A1:F4"/>
     <mergeCell ref="A21:F21"/>
     <mergeCell ref="D5:D6"/>
@@ -16435,12 +16441,6 @@
     <mergeCell ref="D7:D11"/>
     <mergeCell ref="B18:F19"/>
     <mergeCell ref="B7:B11"/>
-    <mergeCell ref="E7:E11"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="B12:B16"/>
-    <mergeCell ref="C7:C11"/>
-    <mergeCell ref="C12:C16"/>
-    <mergeCell ref="A7:A11"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.86614173228346458" right="0.39370078740157483" top="0.70866141732283472" bottom="0.74803149606299213" header="0.31496062992125978" footer="0.31496062992125978"/>

</xml_diff>